<commit_message>
Volviendo al inicio desde obtener excel
</commit_message>
<xml_diff>
--- a/gen_excel/tableros_concurso_125.xlsx
+++ b/gen_excel/tableros_concurso_125.xlsx
@@ -17,24 +17,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>CONCURSANTE</t>
   </si>
   <si>
+    <t>POSICION</t>
+  </si>
+  <si>
     <t>PUNTAJE TOTAL</t>
   </si>
   <si>
     <t>EMPATADO</t>
   </si>
   <si>
-    <t>a</t>
+    <t>Andrew</t>
   </si>
   <si>
     <t>NO</t>
   </si>
   <si>
-    <t>b</t>
+    <t>Daniela</t>
+  </si>
+  <si>
+    <t>RONDA</t>
   </si>
   <si>
     <t>CATEGORIA</t>
@@ -481,16 +487,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -499,12 +508,12 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -513,7 +522,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -537,7 +546,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,191 +558,176 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A2"/>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3"/>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4"/>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5"/>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
+      <c r="A6"/>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
+      <c r="A7"/>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
+      <c r="A8"/>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
+      <c r="A9"/>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
+      <c r="A10"/>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10"/>
       <c r="F10">
@@ -741,37 +735,33 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
+      <c r="A11"/>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F11">
         <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
+      <c r="A12"/>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E12"/>
       <c r="F12">
@@ -779,17 +769,15 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
+      <c r="A13"/>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E13">
         <v>1938</v>
@@ -799,17 +787,15 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
+      <c r="A14"/>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14"/>
       <c r="F14">
@@ -817,37 +803,33 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
+      <c r="A15"/>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F15">
         <v>-2</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
+      <c r="A16"/>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E16"/>
       <c r="F16">
@@ -855,23 +837,89 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
+      <c r="A17"/>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F17">
         <v>-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18"/>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19"/>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20"/>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21"/>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -895,7 +943,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -907,34 +955,37 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F2">
         <v>-1</v>
@@ -942,16 +993,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E3"/>
       <c r="F3">
@@ -960,16 +1011,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E4"/>
       <c r="F4">
@@ -978,39 +1029,21 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5"/>
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
       <c r="F5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6">
         <v>3</v>
       </c>
     </row>

</xml_diff>